<commit_message>
used linear regression to forecast future median incomes (quintile), income gaps and income ratios.
</commit_message>
<xml_diff>
--- a/deciles_income_gap_ratio.xlsx
+++ b/deciles_income_gap_ratio.xlsx
@@ -1592,12 +1592,8 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
-      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1609,12 +1605,8 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
-      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>